<commit_message>
updating dash boad features with class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/classes/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/classes/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="494">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1620,6 +1620,9 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.15-21-01-2022-14:05.apk</t>
   </si>
 </sst>
 </file>
@@ -2064,56 +2067,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16616,22 +16619,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="18" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="18" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="18" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="18" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="18" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="18" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="18" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="18" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="18" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="18" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="18" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="18" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="18" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="18" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="18" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="18" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="18" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="18" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="18" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="18" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16706,21 +16709,28 @@
       <c r="D2" s="22" t="s">
         <v>419</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="22" t="s">
         <v>420</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="22" t="s">
         <v>421</v>
       </c>
       <c r="J2" s="23" t="s">
         <v>422</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="24" t="s">
         <v>423</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="23" t="n">
         <v>500</v>
       </c>
@@ -16744,28 +16754,35 @@
       <c r="D3" s="21" t="s">
         <v>419</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="21" t="s">
         <v>420</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="26" t="s">
         <v>427</v>
       </c>
       <c r="J3" s="26" t="s">
         <v>422</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="24" t="s">
         <v>423</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="23" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="26" t="s">
         <v>425</v>
       </c>
-      <c r="S3" s="27" t="n">
+      <c r="S3" s="27" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16806,7 +16823,7 @@
         <v>436</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>437</v>
+        <v>493</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>438</v>
@@ -16817,13 +16834,14 @@
       <c r="O4" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="23" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S4" s="31" t="n">
+      <c r="S4" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16874,13 +16892,14 @@
       <c r="O5" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="23" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S5" s="31" t="n">
+      <c r="S5" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16916,6 +16935,7 @@
       <c r="J6" s="8" t="s">
         <v>435</v>
       </c>
+      <c r="K6"/>
       <c r="L6" s="11" t="s">
         <v>446</v>
       </c>
@@ -16928,13 +16948,14 @@
       <c r="O6" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="23" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S6" s="31" t="n">
+      <c r="S6" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16970,6 +16991,8 @@
       <c r="J7" s="8" t="s">
         <v>435</v>
       </c>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="11" t="s">
         <v>438</v>
       </c>
@@ -16979,13 +17002,14 @@
       <c r="O7" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="23" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S7" s="31" t="n">
+      <c r="S7" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17024,13 +17048,18 @@
       <c r="K8" s="30" t="s">
         <v>454</v>
       </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="23" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="S8" s="31" t="n">
+      <c r="S8" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17069,18 +17098,30 @@
       <c r="K9" s="34" t="s">
         <v>454</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="23" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="S9" s="31" t="n">
+      <c r="S9" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10" s="33" t="s">
         <v>459</v>
       </c>
@@ -17090,6 +17131,15 @@
       <c r="J10" s="30" t="s">
         <v>453</v>
       </c>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -17133,9 +17183,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updating business class methods and features
</commit_message>
<xml_diff>
--- a/${project.build.directory}/classes/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/classes/test/resources/DataSet/NMCO_ONB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="493">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1620,9 +1620,6 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
-  </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.15-21-01-2022-14:05.apk</t>
   </si>
 </sst>
 </file>
@@ -2059,64 +2056,64 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A162" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B162" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A162" activeCellId="0" sqref="A162"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B165" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A165" activeCellId="0" sqref="A165"/>
       <selection pane="topRight" activeCell="A168" activeCellId="0" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16619,22 +16616,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="18" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="18" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="18" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="18" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="18" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="18" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="18" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="18" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="18" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="18" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="18" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="18" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="18" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="18" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="18" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="18" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="18" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="18" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="18" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="18" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="18" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="18" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="18" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="18" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16709,28 +16706,21 @@
       <c r="D2" s="22" t="s">
         <v>419</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
       <c r="G2" s="22" t="s">
         <v>420</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="22" t="s">
         <v>421</v>
       </c>
       <c r="J2" s="23" t="s">
         <v>422</v>
       </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
       <c r="N2" s="24" t="s">
         <v>423</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="P2"/>
       <c r="Q2" s="23" t="n">
         <v>500</v>
       </c>
@@ -16754,35 +16744,28 @@
       <c r="D3" s="21" t="s">
         <v>419</v>
       </c>
-      <c r="E3"/>
-      <c r="F3"/>
       <c r="G3" s="21" t="s">
         <v>420</v>
       </c>
-      <c r="H3"/>
       <c r="I3" s="26" t="s">
         <v>427</v>
       </c>
       <c r="J3" s="26" t="s">
         <v>422</v>
       </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
       <c r="N3" s="24" t="s">
         <v>423</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="P3"/>
       <c r="Q3" s="23" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="26" t="s">
         <v>425</v>
       </c>
-      <c r="S3" s="27" t="b">
+      <c r="S3" s="27" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16823,7 +16806,7 @@
         <v>436</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>493</v>
+        <v>437</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>438</v>
@@ -16834,14 +16817,13 @@
       <c r="O4" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="P4"/>
       <c r="Q4" s="23" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S4" s="31" t="b">
+      <c r="S4" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16892,14 +16874,13 @@
       <c r="O5" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="P5"/>
       <c r="Q5" s="23" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S5" s="31" t="b">
+      <c r="S5" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16935,7 +16916,6 @@
       <c r="J6" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="K6"/>
       <c r="L6" s="11" t="s">
         <v>446</v>
       </c>
@@ -16948,14 +16928,13 @@
       <c r="O6" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="P6"/>
       <c r="Q6" s="23" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S6" s="31" t="b">
+      <c r="S6" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16991,8 +16970,6 @@
       <c r="J7" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="K7"/>
-      <c r="L7"/>
       <c r="M7" s="11" t="s">
         <v>438</v>
       </c>
@@ -17002,14 +16979,13 @@
       <c r="O7" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="P7"/>
       <c r="Q7" s="23" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S7" s="31" t="b">
+      <c r="S7" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17048,18 +17024,13 @@
       <c r="K8" s="30" t="s">
         <v>454</v>
       </c>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
       <c r="Q8" s="23" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="S8" s="31" t="b">
+      <c r="S8" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17098,30 +17069,18 @@
       <c r="K9" s="34" t="s">
         <v>454</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
       <c r="Q9" s="23" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="S9" s="31" t="b">
+      <c r="S9" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
       <c r="H10" s="33" t="s">
         <v>459</v>
       </c>
@@ -17131,15 +17090,6 @@
       <c r="J10" s="30" t="s">
         <v>453</v>
       </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -17183,9 +17133,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updating entityAddNewUSer feature and objact class
</commit_message>
<xml_diff>
--- a/${project.build.directory}/classes/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/classes/test/resources/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="494">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1338,7 +1338,7 @@
     <t xml:space="preserve">https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.15-21-01-2022-14:05.apk</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation-1-0-15-21-01-2022.apk</t>
+    <t xml:space="preserve">Automation-1-0-16-27-01-2022.apk</t>
   </si>
   <si>
     <t xml:space="preserve">com.iexceed.assistedonboardingapp.assistedonboarding.AssistedOnboardingActivity</t>
@@ -1620,6 +1620,9 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
+  </si>
+  <si>
+    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.16-27-01-2022-10:18.apk</t>
   </si>
 </sst>
 </file>
@@ -2056,64 +2059,64 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B165" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A165" activeCellId="0" sqref="A165"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A159" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B159" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A159" activeCellId="0" sqref="A159"/>
       <selection pane="topRight" activeCell="A168" activeCellId="0" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
+    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
+    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
+    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
+    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
+    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
+    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
+    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
+    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
+    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
+    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
+    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
+    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
+    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
+    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
+    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
+    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
+    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
+    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
+    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
+    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
+    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
+    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16606,32 +16609,32 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M5" activeCellId="0" sqref="M5"/>
+      <selection pane="bottomRight" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="5.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="18" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="18" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="18" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="18" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="18" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="18" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="18" width="26.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="18" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="18" width="29.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="18" width="9.17"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="18" width="12.57" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="18" width="5.18" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="4" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="18" width="19.4" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="18" width="20.5" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="18" width="15.11" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="18" width="18.85" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="18" width="17.86" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="13" customWidth="true" hidden="false" style="18" width="14.87" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="18" width="19.18" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="18" width="26.35" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="17" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="18" width="29.45" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16706,21 +16709,28 @@
       <c r="D2" s="22" t="s">
         <v>419</v>
       </c>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="22" t="s">
         <v>420</v>
       </c>
+      <c r="H2"/>
       <c r="I2" s="22" t="s">
         <v>421</v>
       </c>
       <c r="J2" s="23" t="s">
         <v>422</v>
       </c>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
       <c r="N2" s="24" t="s">
         <v>423</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P2"/>
       <c r="Q2" s="23" t="n">
         <v>500</v>
       </c>
@@ -16744,28 +16754,35 @@
       <c r="D3" s="21" t="s">
         <v>419</v>
       </c>
+      <c r="E3"/>
+      <c r="F3"/>
       <c r="G3" s="21" t="s">
         <v>420</v>
       </c>
+      <c r="H3"/>
       <c r="I3" s="26" t="s">
         <v>427</v>
       </c>
       <c r="J3" s="26" t="s">
         <v>422</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
       <c r="N3" s="24" t="s">
         <v>423</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P3"/>
       <c r="Q3" s="23" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="26" t="s">
         <v>425</v>
       </c>
-      <c r="S3" s="27" t="n">
+      <c r="S3" s="27" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16806,7 +16823,7 @@
         <v>436</v>
       </c>
       <c r="L4" s="18" t="s">
-        <v>437</v>
+        <v>493</v>
       </c>
       <c r="M4" s="11" t="s">
         <v>438</v>
@@ -16817,13 +16834,14 @@
       <c r="O4" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P4"/>
       <c r="Q4" s="23" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S4" s="31" t="n">
+      <c r="S4" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16874,13 +16892,14 @@
       <c r="O5" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P5"/>
       <c r="Q5" s="23" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S5" s="31" t="n">
+      <c r="S5" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16916,6 +16935,7 @@
       <c r="J6" s="8" t="s">
         <v>435</v>
       </c>
+      <c r="K6"/>
       <c r="L6" s="11" t="s">
         <v>446</v>
       </c>
@@ -16928,13 +16948,14 @@
       <c r="O6" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P6"/>
       <c r="Q6" s="23" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S6" s="31" t="n">
+      <c r="S6" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16970,6 +16991,8 @@
       <c r="J7" s="8" t="s">
         <v>435</v>
       </c>
+      <c r="K7"/>
+      <c r="L7"/>
       <c r="M7" s="11" t="s">
         <v>438</v>
       </c>
@@ -16979,13 +17002,14 @@
       <c r="O7" s="11" t="s">
         <v>424</v>
       </c>
+      <c r="P7"/>
       <c r="Q7" s="23" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="S7" s="31" t="n">
+      <c r="S7" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17024,13 +17048,18 @@
       <c r="K8" s="30" t="s">
         <v>454</v>
       </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
       <c r="Q8" s="23" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="S8" s="31" t="n">
+      <c r="S8" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17069,18 +17098,30 @@
       <c r="K9" s="34" t="s">
         <v>454</v>
       </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
       <c r="Q9" s="23" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="S9" s="31" t="n">
+      <c r="S9" s="31" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
       <c r="H10" s="33" t="s">
         <v>459</v>
       </c>
@@ -17090,6 +17131,15 @@
       <c r="J10" s="30" t="s">
         <v>453</v>
       </c>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -17133,9 +17183,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updating business location feature file
</commit_message>
<xml_diff>
--- a/${project.build.directory}/classes/test/resources/DataSet/NMCO_ONB.xlsx
+++ b/${project.build.directory}/classes/test/resources/DataSet/NMCO_ONB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="497">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -1222,6 +1222,18 @@
   </si>
   <si>
     <t xml:space="preserve">TestCase_164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BusinessLocation TypeOfOpeartion-invalid inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BusinessLocation TypeOfOpeartion-invalid inputs-Arabic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_166</t>
   </si>
   <si>
     <t xml:space="preserve">mode</t>
@@ -1620,9 +1632,6 @@
       </rPr>
       <t xml:space="preserve">);</t>
     </r>
-  </si>
-  <si>
-    <t>https://artifactory.appzillon.com/artifactory/android-apk/ao/manual/qaRelease-1.0.16-27-01-2022-10:18.apk</t>
   </si>
 </sst>
 </file>
@@ -2059,64 +2068,64 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A159" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B159" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A159" activeCellId="0" sqref="A159"/>
-      <selection pane="topRight" activeCell="A168" activeCellId="0" sqref="A168"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A165" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B165" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A165" activeCellId="0" sqref="A165"/>
+      <selection pane="topRight" activeCell="B169" activeCellId="0" sqref="B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="32.3" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="12.85" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="4.43" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="7.83" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="6" customWidth="true" hidden="false" style="1" width="11.9" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="8" customWidth="true" hidden="false" style="1" width="15.54" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="17.31" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="2" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.2" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="15.21" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="true" hidden="false" style="1" width="13.78" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="13.56" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="24.43" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="19" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="20" max="20" customWidth="true" hidden="false" style="1" width="14.11" collapsed="true" outlineLevel="0"/>
-    <col min="21" max="21" customWidth="true" hidden="false" style="2" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="22" max="22" customWidth="true" hidden="false" style="2" width="21.17" collapsed="true" outlineLevel="0"/>
-    <col min="23" max="23" customWidth="true" hidden="false" style="1" width="14.99" collapsed="true" outlineLevel="0"/>
-    <col min="24" max="25" customWidth="true" hidden="false" style="1" width="19.51" collapsed="true" outlineLevel="0"/>
-    <col min="26" max="26" customWidth="true" hidden="false" style="1" width="24.36" collapsed="true" outlineLevel="0"/>
-    <col min="27" max="27" customWidth="true" hidden="false" style="1" width="13.0" collapsed="true" outlineLevel="0"/>
-    <col min="28" max="28" customWidth="true" hidden="false" style="1" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="29" max="29" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="30" max="31" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="32" max="32" customWidth="true" hidden="false" style="1" width="22.49" collapsed="true" outlineLevel="0"/>
-    <col min="33" max="33" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="34" max="34" customWidth="true" hidden="false" style="1" width="20.28" collapsed="true" outlineLevel="0"/>
-    <col min="35" max="35" customWidth="true" hidden="false" style="1" width="21.04" collapsed="true" outlineLevel="0"/>
-    <col min="36" max="37" customWidth="true" hidden="false" style="1" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="38" max="38" customWidth="true" hidden="false" style="1" width="18.3" collapsed="true" outlineLevel="0"/>
-    <col min="39" max="39" customWidth="true" hidden="false" style="1" width="19.95" collapsed="true" outlineLevel="0"/>
-    <col min="40" max="40" customWidth="true" hidden="false" style="2" width="20.84" collapsed="true" outlineLevel="0"/>
-    <col min="41" max="41" customWidth="true" hidden="false" style="3" width="32.74" collapsed="true" outlineLevel="0"/>
-    <col min="42" max="42" customWidth="true" hidden="false" style="1" width="22.04" collapsed="true" outlineLevel="0"/>
-    <col min="43" max="43" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="44" max="44" customWidth="true" hidden="false" style="1" width="20.94" collapsed="true" outlineLevel="0"/>
-    <col min="45" max="45" customWidth="true" hidden="false" style="1" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="46" max="46" customWidth="true" hidden="false" style="1" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="47" max="47" customWidth="true" hidden="false" style="1" width="16.74" collapsed="true" outlineLevel="0"/>
-    <col min="48" max="48" customWidth="true" hidden="false" style="3" width="14.0" collapsed="true" outlineLevel="0"/>
-    <col min="49" max="49" customWidth="true" hidden="false" style="3" width="16.11" collapsed="true" outlineLevel="0"/>
-    <col min="50" max="50" customWidth="true" hidden="false" style="1" width="12.35" collapsed="true" outlineLevel="0"/>
-    <col min="51" max="52" customWidth="true" hidden="false" style="1" width="17.64" collapsed="true" outlineLevel="0"/>
-    <col min="53" max="53" customWidth="true" hidden="false" style="1" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="54" max="54" customWidth="true" hidden="false" style="2" width="18.08" collapsed="true" outlineLevel="0"/>
-    <col min="55" max="990" customWidth="true" hidden="false" style="1" width="8.57" collapsed="true" outlineLevel="0"/>
-    <col min="991" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="1" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="18.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="2" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="3" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="20.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="51" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="2" width="18.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="990" min="55" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="991" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16465,7 +16474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
         <v>396</v>
       </c>
@@ -16533,6 +16542,148 @@
         <v>382</v>
       </c>
       <c r="AB168" s="16" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="C169" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E169" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G169" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="H169" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="I169" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J169" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K169" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M169" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N169" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O169" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P169" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q169" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="R169" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="S169" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="T169" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="U169" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="V169" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z169" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="AA169" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="AB169" s="16" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E170" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G170" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="H170" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="I170" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J170" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K170" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M170" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N170" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O170" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P170" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q170" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="R170" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="S170" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="T170" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="U170" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="V170" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z170" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="AA170" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="AB170" s="16" t="n">
         <v>12</v>
       </c>
     </row>
@@ -16591,6 +16742,8 @@
     <hyperlink ref="I162" r:id="rId50" display="parkjimin@gmail.com"/>
     <hyperlink ref="I167" r:id="rId51" display="parkjimin@gmail.com"/>
     <hyperlink ref="I168" r:id="rId52" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I169" r:id="rId53" display="parkjimin@gmail.com"/>
+    <hyperlink ref="I170" r:id="rId54" display="parkjimin@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -16609,32 +16762,32 @@
   </sheetPr>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
       <selection pane="bottomRight" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="18" width="12.57" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="18" width="5.18" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="4" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="18" width="19.4" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="18" width="20.5" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="18" width="15.11" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="18" width="18.85" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="18" width="17.86" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="13" customWidth="true" hidden="false" style="18" width="14.87" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="18" width="19.18" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="18" width="26.35" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="17" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="18" width="29.45" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="true" hidden="false" style="18" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="5.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="18" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="18" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="18" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="18" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="18" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="18" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="18" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="18" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="18" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="18" width="19.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="18" width="26.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="18" width="9.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="18" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="18" width="9.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16645,97 +16798,90 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="R1" s="20" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>419</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2"/>
+        <v>423</v>
+      </c>
       <c r="G2" s="22" t="s">
-        <v>420</v>
-      </c>
-      <c r="H2"/>
+        <v>424</v>
+      </c>
       <c r="I2" s="22" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>422</v>
-      </c>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
+        <v>426</v>
+      </c>
       <c r="N2" s="24" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="P2"/>
+        <v>428</v>
+      </c>
       <c r="Q2" s="23" t="n">
         <v>500</v>
       </c>
       <c r="R2" s="25" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="S2" s="23" t="n">
         <v>0</v>
@@ -16743,46 +16889,39 @@
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>426</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>418</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>419</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3" s="21" t="s">
-        <v>420</v>
-      </c>
-      <c r="H3"/>
-      <c r="I3" s="26" t="s">
+      <c r="N3" s="24" t="s">
         <v>427</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>422</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3" s="24" t="s">
-        <v>423</v>
-      </c>
       <c r="O3" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="P3"/>
+        <v>428</v>
+      </c>
       <c r="Q3" s="23" t="n">
         <v>501</v>
       </c>
       <c r="R3" s="26" t="s">
-        <v>425</v>
-      </c>
-      <c r="S3" s="27" t="b">
+        <v>429</v>
+      </c>
+      <c r="S3" s="27" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -16790,356 +16929,323 @@
     </row>
     <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>438</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>443</v>
+      </c>
+      <c r="O4" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>430</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>431</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>432</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>434</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>493</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>438</v>
-      </c>
-      <c r="N4" s="24" t="s">
-        <v>439</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="P4"/>
       <c r="Q4" s="23" t="n">
         <v>502</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="S4" s="31" t="b">
+        <v>444</v>
+      </c>
+      <c r="S4" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>448</v>
+      </c>
+      <c r="M5" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="N5" s="24" t="s">
         <v>443</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>444</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>438</v>
-      </c>
-      <c r="N5" s="24" t="s">
-        <v>439</v>
-      </c>
       <c r="O5" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="P5"/>
+        <v>428</v>
+      </c>
       <c r="Q5" s="23" t="n">
         <v>503</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="S5" s="31" t="b">
+        <v>444</v>
+      </c>
+      <c r="S5" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="K6"/>
+        <v>439</v>
+      </c>
       <c r="L6" s="11" t="s">
-        <v>493</v>
+        <v>450</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="N6" s="24" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="P6"/>
+        <v>428</v>
+      </c>
       <c r="Q6" s="23" t="n">
         <v>504</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="S6" s="31" t="b">
+        <v>444</v>
+      </c>
+      <c r="S6" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7"/>
+        <v>439</v>
+      </c>
       <c r="M7" s="11" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="P7"/>
+        <v>428</v>
+      </c>
       <c r="Q7" s="23" t="n">
         <v>505</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="S7" s="31" t="b">
+        <v>444</v>
+      </c>
+      <c r="S7" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="K8" s="30" t="s">
-        <v>454</v>
-      </c>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
+        <v>458</v>
+      </c>
       <c r="Q8" s="23" t="n">
         <v>506</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>455</v>
-      </c>
-      <c r="S8" s="31" t="b">
+        <v>459</v>
+      </c>
+      <c r="S8" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="82.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="H9" s="33" t="s">
+        <v>461</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="J9" s="30" t="s">
         <v>457</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="K9" s="34" t="s">
         <v>458</v>
       </c>
-      <c r="J9" s="30" t="s">
-        <v>453</v>
-      </c>
-      <c r="K9" s="34" t="s">
-        <v>454</v>
-      </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
       <c r="Q9" s="23" t="n">
         <v>507</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>455</v>
-      </c>
-      <c r="S9" s="31" t="b">
+        <v>459</v>
+      </c>
+      <c r="S9" s="31" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
       <c r="H10" s="33" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>453</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
+        <v>457</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -17183,69 +17289,69 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="13.93" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="true" hidden="false" style="0" width="9.14" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="35" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="35" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="35" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="35" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="35" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="35" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="35" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -17254,139 +17360,139 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="36" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="F25" s="36" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="9" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="36" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="36" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="37" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="38" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>